<commit_message>
fixed some html and css errors.
</commit_message>
<xml_diff>
--- a/public/import_template_author_year.xlsx
+++ b/public/import_template_author_year.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="import_template_author_year.csv" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,6 @@
     <t>user_id</t>
   </si>
   <si>
-    <t>coral_id</t>
-  </si>
-  <si>
     <t>location_id</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>notes</t>
+  </si>
+  <si>
+    <t>specie_id</t>
   </si>
 </sst>
 </file>
@@ -437,7 +437,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
@@ -452,43 +454,43 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>